<commit_message>
updated payroll dashboard with modal update
</commit_message>
<xml_diff>
--- a/public/extra/import_file/payroll_report.xlsx
+++ b/public/extra/import_file/payroll_report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="43">
   <si>
     <t>ID</t>
   </si>
@@ -59,6 +59,9 @@
     <t>Net Amount</t>
   </si>
   <si>
+    <t>(Normal Payroll) - 'Both'</t>
+  </si>
+  <si>
     <t>Qweqwewq, Qweqweq Qwe</t>
   </si>
   <si>
@@ -111,6 +114,36 @@
   </si>
   <si>
     <t>Vv4, Cc Sdd</t>
+  </si>
+  <si>
+    <t>09-30-2019</t>
+  </si>
+  <si>
+    <t>7,153.85</t>
+  </si>
+  <si>
+    <t>7,384.62</t>
+  </si>
+  <si>
+    <t>-1,484.62</t>
+  </si>
+  <si>
+    <t>(Normal Payroll) - 'Rank And File'</t>
+  </si>
+  <si>
+    <t>09-29-2019</t>
+  </si>
+  <si>
+    <t>(13th Month) - 'Both'</t>
+  </si>
+  <si>
+    <t>12,000.00</t>
+  </si>
+  <si>
+    <t>2,400.00</t>
+  </si>
+  <si>
+    <t>9,600.00</t>
   </si>
 </sst>
 </file>
@@ -449,7 +482,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:N49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="I26" sqref="I26"/>
@@ -502,70 +535,31 @@
       </c>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" t="s">
         <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2">
-        <v>436</v>
-      </c>
-      <c r="I2">
-        <v>330</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H3">
         <v>436</v>
@@ -586,62 +580,62 @@
         <v>0</v>
       </c>
       <c r="N3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4">
+        <v>436</v>
+      </c>
+      <c r="I4">
+        <v>330</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4" t="s">
         <v>22</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>137.5</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>-137.5</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -679,13 +673,13 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -723,13 +717,13 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -767,13 +761,13 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -811,13 +805,13 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -855,13 +849,13 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -879,7 +873,7 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>137.5</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -894,18 +888,18 @@
         <v>0</v>
       </c>
       <c r="N10">
-        <v>0</v>
+        <v>-137.5</v>
       </c>
     </row>
     <row r="11" spans="1:14">
       <c r="A11">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
         <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -943,13 +937,13 @@
     </row>
     <row r="12" spans="1:14">
       <c r="A12">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
         <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -987,45 +981,1512 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
         <v>31</v>
       </c>
       <c r="C13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
         <v>15</v>
       </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13">
+      <c r="C16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>100</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17" t="s">
+        <v>35</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>100</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20">
+        <v>6</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22">
+        <v>8</v>
+      </c>
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23">
+        <v>9</v>
+      </c>
+      <c r="B23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24">
+        <v>21</v>
+      </c>
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25">
+        <v>22</v>
+      </c>
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26">
+        <v>23</v>
+      </c>
+      <c r="B26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27">
+        <v>24</v>
+      </c>
+      <c r="B27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29" t="s">
+        <v>19</v>
+      </c>
+      <c r="H29">
+        <v>436</v>
+      </c>
+      <c r="I29">
+        <v>330</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <v>0</v>
+      </c>
+      <c r="N29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30">
+        <v>2</v>
+      </c>
+      <c r="B30" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30" t="s">
+        <v>21</v>
+      </c>
+      <c r="H30">
+        <v>436</v>
+      </c>
+      <c r="I30">
+        <v>330</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="L30">
+        <v>0</v>
+      </c>
+      <c r="M30">
+        <v>0</v>
+      </c>
+      <c r="N30" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31">
+        <v>4</v>
+      </c>
+      <c r="B31" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>137.5</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <v>-137.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32">
+        <v>5</v>
+      </c>
+      <c r="B32" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>137.5</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
+      <c r="M32">
+        <v>0</v>
+      </c>
+      <c r="N32">
+        <v>-137.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
+      <c r="A33">
+        <v>6</v>
+      </c>
+      <c r="B33" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" t="s">
+        <v>38</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>137.5</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
+      <c r="M33">
+        <v>0</v>
+      </c>
+      <c r="N33">
+        <v>-137.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
+      <c r="A34">
+        <v>7</v>
+      </c>
+      <c r="B34" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" t="s">
+        <v>38</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>137.5</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <v>0</v>
+      </c>
+      <c r="L34">
+        <v>0</v>
+      </c>
+      <c r="M34">
+        <v>0</v>
+      </c>
+      <c r="N34">
+        <v>-137.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
+      <c r="A35">
+        <v>8</v>
+      </c>
+      <c r="B35" t="s">
+        <v>27</v>
+      </c>
+      <c r="C35" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>137.5</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+      <c r="N35">
+        <v>-137.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
+      <c r="A36">
+        <v>9</v>
+      </c>
+      <c r="B36" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>137.5</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <v>0</v>
+      </c>
+      <c r="L36">
+        <v>0</v>
+      </c>
+      <c r="M36">
+        <v>0</v>
+      </c>
+      <c r="N36">
+        <v>-137.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="A37" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" t="s">
+        <v>33</v>
+      </c>
+      <c r="D38" t="s">
+        <v>40</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
+      <c r="K38" t="s">
+        <v>41</v>
+      </c>
+      <c r="L38">
+        <v>0</v>
+      </c>
+      <c r="M38">
+        <v>0</v>
+      </c>
+      <c r="N38" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
+      <c r="A39">
+        <v>2</v>
+      </c>
+      <c r="B39" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" t="s">
+        <v>33</v>
+      </c>
+      <c r="D39" t="s">
+        <v>40</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39">
+        <v>0</v>
+      </c>
+      <c r="K39" t="s">
+        <v>41</v>
+      </c>
+      <c r="L39">
+        <v>0</v>
+      </c>
+      <c r="M39">
+        <v>0</v>
+      </c>
+      <c r="N39" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="A40">
+        <v>4</v>
+      </c>
+      <c r="B40" t="s">
+        <v>23</v>
+      </c>
+      <c r="C40" t="s">
+        <v>33</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
+      <c r="L40">
+        <v>0</v>
+      </c>
+      <c r="M40">
+        <v>0</v>
+      </c>
+      <c r="N40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="A41">
+        <v>5</v>
+      </c>
+      <c r="B41" t="s">
+        <v>24</v>
+      </c>
+      <c r="C41" t="s">
+        <v>33</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+      <c r="K41">
+        <v>0</v>
+      </c>
+      <c r="L41">
+        <v>0</v>
+      </c>
+      <c r="M41">
+        <v>0</v>
+      </c>
+      <c r="N41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
+      <c r="A42">
+        <v>6</v>
+      </c>
+      <c r="B42" t="s">
+        <v>25</v>
+      </c>
+      <c r="C42" t="s">
+        <v>33</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
+      <c r="K42">
+        <v>0</v>
+      </c>
+      <c r="L42">
+        <v>0</v>
+      </c>
+      <c r="M42">
+        <v>0</v>
+      </c>
+      <c r="N42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14">
+      <c r="A43">
+        <v>7</v>
+      </c>
+      <c r="B43" t="s">
+        <v>26</v>
+      </c>
+      <c r="C43" t="s">
+        <v>33</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <v>0</v>
+      </c>
+      <c r="L43">
+        <v>0</v>
+      </c>
+      <c r="M43">
+        <v>0</v>
+      </c>
+      <c r="N43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14">
+      <c r="A44">
+        <v>8</v>
+      </c>
+      <c r="B44" t="s">
+        <v>27</v>
+      </c>
+      <c r="C44" t="s">
+        <v>33</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <v>0</v>
+      </c>
+      <c r="L44">
+        <v>0</v>
+      </c>
+      <c r="M44">
+        <v>0</v>
+      </c>
+      <c r="N44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14">
+      <c r="A45">
+        <v>9</v>
+      </c>
+      <c r="B45" t="s">
+        <v>28</v>
+      </c>
+      <c r="C45" t="s">
+        <v>33</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>0</v>
+      </c>
+      <c r="L45">
+        <v>0</v>
+      </c>
+      <c r="M45">
+        <v>0</v>
+      </c>
+      <c r="N45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14">
+      <c r="A46">
+        <v>21</v>
+      </c>
+      <c r="B46" t="s">
+        <v>29</v>
+      </c>
+      <c r="C46" t="s">
+        <v>33</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+      <c r="K46">
+        <v>0</v>
+      </c>
+      <c r="L46">
+        <v>0</v>
+      </c>
+      <c r="M46">
+        <v>0</v>
+      </c>
+      <c r="N46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14">
+      <c r="A47">
+        <v>22</v>
+      </c>
+      <c r="B47" t="s">
+        <v>30</v>
+      </c>
+      <c r="C47" t="s">
+        <v>33</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+      <c r="K47">
+        <v>0</v>
+      </c>
+      <c r="L47">
+        <v>0</v>
+      </c>
+      <c r="M47">
+        <v>0</v>
+      </c>
+      <c r="N47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14">
+      <c r="A48">
+        <v>23</v>
+      </c>
+      <c r="B48" t="s">
+        <v>31</v>
+      </c>
+      <c r="C48" t="s">
+        <v>33</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+      <c r="K48">
+        <v>0</v>
+      </c>
+      <c r="L48">
+        <v>0</v>
+      </c>
+      <c r="M48">
+        <v>0</v>
+      </c>
+      <c r="N48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14">
+      <c r="A49">
+        <v>24</v>
+      </c>
+      <c r="B49" t="s">
+        <v>32</v>
+      </c>
+      <c r="C49" t="s">
+        <v>33</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49">
+        <v>0</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
+      </c>
+      <c r="K49">
+        <v>0</v>
+      </c>
+      <c r="L49">
+        <v>0</v>
+      </c>
+      <c r="M49">
+        <v>0</v>
+      </c>
+      <c r="N49">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
no changes...edited but reverted
</commit_message>
<xml_diff>
--- a/public/extra/import_file/payroll_report.xlsx
+++ b/public/extra/import_file/payroll_report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="43">
   <si>
     <t>ID</t>
   </si>
@@ -59,6 +59,9 @@
     <t>Net Amount</t>
   </si>
   <si>
+    <t>(Normal Payroll) - 'Both'</t>
+  </si>
+  <si>
     <t>Qweqwewq, Qweqweq Qwe</t>
   </si>
   <si>
@@ -111,6 +114,36 @@
   </si>
   <si>
     <t>Vv4, Cc Sdd</t>
+  </si>
+  <si>
+    <t>09-30-2019</t>
+  </si>
+  <si>
+    <t>7,153.85</t>
+  </si>
+  <si>
+    <t>7,384.62</t>
+  </si>
+  <si>
+    <t>-1,484.62</t>
+  </si>
+  <si>
+    <t>(Normal Payroll) - 'Rank And File'</t>
+  </si>
+  <si>
+    <t>09-29-2019</t>
+  </si>
+  <si>
+    <t>(13th Month) - 'Both'</t>
+  </si>
+  <si>
+    <t>12,000.00</t>
+  </si>
+  <si>
+    <t>2,400.00</t>
+  </si>
+  <si>
+    <t>9,600.00</t>
   </si>
 </sst>
 </file>
@@ -449,7 +482,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:N49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="I26" sqref="I26"/>
@@ -502,70 +535,31 @@
       </c>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" t="s">
         <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2">
-        <v>436</v>
-      </c>
-      <c r="I2">
-        <v>330</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H3">
         <v>436</v>
@@ -586,62 +580,62 @@
         <v>0</v>
       </c>
       <c r="N3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4">
+        <v>436</v>
+      </c>
+      <c r="I4">
+        <v>330</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4" t="s">
         <v>22</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>137.5</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>-137.5</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -679,13 +673,13 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -723,13 +717,13 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -767,13 +761,13 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -811,13 +805,13 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -855,13 +849,13 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -879,7 +873,7 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>137.5</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -894,18 +888,18 @@
         <v>0</v>
       </c>
       <c r="N10">
-        <v>0</v>
+        <v>-137.5</v>
       </c>
     </row>
     <row r="11" spans="1:14">
       <c r="A11">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
         <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -943,13 +937,13 @@
     </row>
     <row r="12" spans="1:14">
       <c r="A12">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
         <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -987,45 +981,1512 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
         <v>31</v>
       </c>
       <c r="C13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
         <v>15</v>
       </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13">
+      <c r="C16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>100</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17" t="s">
+        <v>35</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>100</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20">
+        <v>6</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22">
+        <v>8</v>
+      </c>
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23">
+        <v>9</v>
+      </c>
+      <c r="B23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24">
+        <v>21</v>
+      </c>
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25">
+        <v>22</v>
+      </c>
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26">
+        <v>23</v>
+      </c>
+      <c r="B26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27">
+        <v>24</v>
+      </c>
+      <c r="B27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29" t="s">
+        <v>19</v>
+      </c>
+      <c r="H29">
+        <v>436</v>
+      </c>
+      <c r="I29">
+        <v>330</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <v>0</v>
+      </c>
+      <c r="N29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30">
+        <v>2</v>
+      </c>
+      <c r="B30" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30" t="s">
+        <v>21</v>
+      </c>
+      <c r="H30">
+        <v>436</v>
+      </c>
+      <c r="I30">
+        <v>330</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="L30">
+        <v>0</v>
+      </c>
+      <c r="M30">
+        <v>0</v>
+      </c>
+      <c r="N30" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31">
+        <v>4</v>
+      </c>
+      <c r="B31" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>137.5</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <v>-137.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32">
+        <v>5</v>
+      </c>
+      <c r="B32" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>137.5</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
+      <c r="M32">
+        <v>0</v>
+      </c>
+      <c r="N32">
+        <v>-137.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
+      <c r="A33">
+        <v>6</v>
+      </c>
+      <c r="B33" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" t="s">
+        <v>38</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>137.5</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
+      <c r="M33">
+        <v>0</v>
+      </c>
+      <c r="N33">
+        <v>-137.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
+      <c r="A34">
+        <v>7</v>
+      </c>
+      <c r="B34" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" t="s">
+        <v>38</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>137.5</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <v>0</v>
+      </c>
+      <c r="L34">
+        <v>0</v>
+      </c>
+      <c r="M34">
+        <v>0</v>
+      </c>
+      <c r="N34">
+        <v>-137.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
+      <c r="A35">
+        <v>8</v>
+      </c>
+      <c r="B35" t="s">
+        <v>27</v>
+      </c>
+      <c r="C35" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>137.5</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+      <c r="N35">
+        <v>-137.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
+      <c r="A36">
+        <v>9</v>
+      </c>
+      <c r="B36" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>137.5</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <v>0</v>
+      </c>
+      <c r="L36">
+        <v>0</v>
+      </c>
+      <c r="M36">
+        <v>0</v>
+      </c>
+      <c r="N36">
+        <v>-137.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="A37" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" t="s">
+        <v>33</v>
+      </c>
+      <c r="D38" t="s">
+        <v>40</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
+      <c r="K38" t="s">
+        <v>41</v>
+      </c>
+      <c r="L38">
+        <v>0</v>
+      </c>
+      <c r="M38">
+        <v>0</v>
+      </c>
+      <c r="N38" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
+      <c r="A39">
+        <v>2</v>
+      </c>
+      <c r="B39" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" t="s">
+        <v>33</v>
+      </c>
+      <c r="D39" t="s">
+        <v>40</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39">
+        <v>0</v>
+      </c>
+      <c r="K39" t="s">
+        <v>41</v>
+      </c>
+      <c r="L39">
+        <v>0</v>
+      </c>
+      <c r="M39">
+        <v>0</v>
+      </c>
+      <c r="N39" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="A40">
+        <v>4</v>
+      </c>
+      <c r="B40" t="s">
+        <v>23</v>
+      </c>
+      <c r="C40" t="s">
+        <v>33</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
+      <c r="L40">
+        <v>0</v>
+      </c>
+      <c r="M40">
+        <v>0</v>
+      </c>
+      <c r="N40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="A41">
+        <v>5</v>
+      </c>
+      <c r="B41" t="s">
+        <v>24</v>
+      </c>
+      <c r="C41" t="s">
+        <v>33</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+      <c r="K41">
+        <v>0</v>
+      </c>
+      <c r="L41">
+        <v>0</v>
+      </c>
+      <c r="M41">
+        <v>0</v>
+      </c>
+      <c r="N41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
+      <c r="A42">
+        <v>6</v>
+      </c>
+      <c r="B42" t="s">
+        <v>25</v>
+      </c>
+      <c r="C42" t="s">
+        <v>33</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
+      <c r="K42">
+        <v>0</v>
+      </c>
+      <c r="L42">
+        <v>0</v>
+      </c>
+      <c r="M42">
+        <v>0</v>
+      </c>
+      <c r="N42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14">
+      <c r="A43">
+        <v>7</v>
+      </c>
+      <c r="B43" t="s">
+        <v>26</v>
+      </c>
+      <c r="C43" t="s">
+        <v>33</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <v>0</v>
+      </c>
+      <c r="L43">
+        <v>0</v>
+      </c>
+      <c r="M43">
+        <v>0</v>
+      </c>
+      <c r="N43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14">
+      <c r="A44">
+        <v>8</v>
+      </c>
+      <c r="B44" t="s">
+        <v>27</v>
+      </c>
+      <c r="C44" t="s">
+        <v>33</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <v>0</v>
+      </c>
+      <c r="L44">
+        <v>0</v>
+      </c>
+      <c r="M44">
+        <v>0</v>
+      </c>
+      <c r="N44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14">
+      <c r="A45">
+        <v>9</v>
+      </c>
+      <c r="B45" t="s">
+        <v>28</v>
+      </c>
+      <c r="C45" t="s">
+        <v>33</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>0</v>
+      </c>
+      <c r="L45">
+        <v>0</v>
+      </c>
+      <c r="M45">
+        <v>0</v>
+      </c>
+      <c r="N45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14">
+      <c r="A46">
+        <v>21</v>
+      </c>
+      <c r="B46" t="s">
+        <v>29</v>
+      </c>
+      <c r="C46" t="s">
+        <v>33</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+      <c r="K46">
+        <v>0</v>
+      </c>
+      <c r="L46">
+        <v>0</v>
+      </c>
+      <c r="M46">
+        <v>0</v>
+      </c>
+      <c r="N46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14">
+      <c r="A47">
+        <v>22</v>
+      </c>
+      <c r="B47" t="s">
+        <v>30</v>
+      </c>
+      <c r="C47" t="s">
+        <v>33</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+      <c r="K47">
+        <v>0</v>
+      </c>
+      <c r="L47">
+        <v>0</v>
+      </c>
+      <c r="M47">
+        <v>0</v>
+      </c>
+      <c r="N47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14">
+      <c r="A48">
+        <v>23</v>
+      </c>
+      <c r="B48" t="s">
+        <v>31</v>
+      </c>
+      <c r="C48" t="s">
+        <v>33</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+      <c r="K48">
+        <v>0</v>
+      </c>
+      <c r="L48">
+        <v>0</v>
+      </c>
+      <c r="M48">
+        <v>0</v>
+      </c>
+      <c r="N48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14">
+      <c r="A49">
+        <v>24</v>
+      </c>
+      <c r="B49" t="s">
+        <v>32</v>
+      </c>
+      <c r="C49" t="s">
+        <v>33</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49">
+        <v>0</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
+      </c>
+      <c r="K49">
+        <v>0</v>
+      </c>
+      <c r="L49">
+        <v>0</v>
+      </c>
+      <c r="M49">
+        <v>0</v>
+      </c>
+      <c r="N49">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added partial audit page ui
</commit_message>
<xml_diff>
--- a/public/extra/import_file/payroll_report.xlsx
+++ b/public/extra/import_file/payroll_report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="43">
   <si>
     <t>ID</t>
   </si>
@@ -59,6 +59,9 @@
     <t>Net Amount</t>
   </si>
   <si>
+    <t>(Normal Payroll) - 'Both'</t>
+  </si>
+  <si>
     <t>Qweqwewq, Qweqweq Qwe</t>
   </si>
   <si>
@@ -111,6 +114,36 @@
   </si>
   <si>
     <t>Vv4, Cc Sdd</t>
+  </si>
+  <si>
+    <t>09-30-2019</t>
+  </si>
+  <si>
+    <t>7,153.85</t>
+  </si>
+  <si>
+    <t>7,384.62</t>
+  </si>
+  <si>
+    <t>-1,484.62</t>
+  </si>
+  <si>
+    <t>(Normal Payroll) - 'Rank And File'</t>
+  </si>
+  <si>
+    <t>09-29-2019</t>
+  </si>
+  <si>
+    <t>(13th Month) - 'Both'</t>
+  </si>
+  <si>
+    <t>12,000.00</t>
+  </si>
+  <si>
+    <t>2,400.00</t>
+  </si>
+  <si>
+    <t>9,600.00</t>
   </si>
 </sst>
 </file>
@@ -449,7 +482,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:N49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="I26" sqref="I26"/>
@@ -502,70 +535,31 @@
       </c>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" t="s">
         <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2">
-        <v>436</v>
-      </c>
-      <c r="I2">
-        <v>330</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H3">
         <v>436</v>
@@ -586,62 +580,62 @@
         <v>0</v>
       </c>
       <c r="N3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4">
+        <v>436</v>
+      </c>
+      <c r="I4">
+        <v>330</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4" t="s">
         <v>22</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>137.5</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>-137.5</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -679,13 +673,13 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -723,13 +717,13 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -767,13 +761,13 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -811,13 +805,13 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -855,13 +849,13 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -879,7 +873,7 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>137.5</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -894,18 +888,18 @@
         <v>0</v>
       </c>
       <c r="N10">
-        <v>0</v>
+        <v>-137.5</v>
       </c>
     </row>
     <row r="11" spans="1:14">
       <c r="A11">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
         <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -943,13 +937,13 @@
     </row>
     <row r="12" spans="1:14">
       <c r="A12">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
         <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -987,45 +981,1512 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
         <v>31</v>
       </c>
       <c r="C13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
         <v>15</v>
       </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13">
+      <c r="C16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>100</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17" t="s">
+        <v>35</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>100</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20">
+        <v>6</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22">
+        <v>8</v>
+      </c>
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23">
+        <v>9</v>
+      </c>
+      <c r="B23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24">
+        <v>21</v>
+      </c>
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25">
+        <v>22</v>
+      </c>
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26">
+        <v>23</v>
+      </c>
+      <c r="B26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27">
+        <v>24</v>
+      </c>
+      <c r="B27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29" t="s">
+        <v>19</v>
+      </c>
+      <c r="H29">
+        <v>436</v>
+      </c>
+      <c r="I29">
+        <v>330</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <v>0</v>
+      </c>
+      <c r="N29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30">
+        <v>2</v>
+      </c>
+      <c r="B30" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30" t="s">
+        <v>21</v>
+      </c>
+      <c r="H30">
+        <v>436</v>
+      </c>
+      <c r="I30">
+        <v>330</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="L30">
+        <v>0</v>
+      </c>
+      <c r="M30">
+        <v>0</v>
+      </c>
+      <c r="N30" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31">
+        <v>4</v>
+      </c>
+      <c r="B31" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>137.5</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <v>-137.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32">
+        <v>5</v>
+      </c>
+      <c r="B32" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>137.5</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
+      <c r="M32">
+        <v>0</v>
+      </c>
+      <c r="N32">
+        <v>-137.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
+      <c r="A33">
+        <v>6</v>
+      </c>
+      <c r="B33" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" t="s">
+        <v>38</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>137.5</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
+      <c r="M33">
+        <v>0</v>
+      </c>
+      <c r="N33">
+        <v>-137.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
+      <c r="A34">
+        <v>7</v>
+      </c>
+      <c r="B34" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" t="s">
+        <v>38</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>137.5</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <v>0</v>
+      </c>
+      <c r="L34">
+        <v>0</v>
+      </c>
+      <c r="M34">
+        <v>0</v>
+      </c>
+      <c r="N34">
+        <v>-137.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
+      <c r="A35">
+        <v>8</v>
+      </c>
+      <c r="B35" t="s">
+        <v>27</v>
+      </c>
+      <c r="C35" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>137.5</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+      <c r="N35">
+        <v>-137.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
+      <c r="A36">
+        <v>9</v>
+      </c>
+      <c r="B36" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>137.5</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <v>0</v>
+      </c>
+      <c r="L36">
+        <v>0</v>
+      </c>
+      <c r="M36">
+        <v>0</v>
+      </c>
+      <c r="N36">
+        <v>-137.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="A37" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" t="s">
+        <v>33</v>
+      </c>
+      <c r="D38" t="s">
+        <v>40</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
+      <c r="K38" t="s">
+        <v>41</v>
+      </c>
+      <c r="L38">
+        <v>0</v>
+      </c>
+      <c r="M38">
+        <v>0</v>
+      </c>
+      <c r="N38" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
+      <c r="A39">
+        <v>2</v>
+      </c>
+      <c r="B39" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" t="s">
+        <v>33</v>
+      </c>
+      <c r="D39" t="s">
+        <v>40</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39">
+        <v>0</v>
+      </c>
+      <c r="K39" t="s">
+        <v>41</v>
+      </c>
+      <c r="L39">
+        <v>0</v>
+      </c>
+      <c r="M39">
+        <v>0</v>
+      </c>
+      <c r="N39" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="A40">
+        <v>4</v>
+      </c>
+      <c r="B40" t="s">
+        <v>23</v>
+      </c>
+      <c r="C40" t="s">
+        <v>33</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
+      <c r="L40">
+        <v>0</v>
+      </c>
+      <c r="M40">
+        <v>0</v>
+      </c>
+      <c r="N40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="A41">
+        <v>5</v>
+      </c>
+      <c r="B41" t="s">
+        <v>24</v>
+      </c>
+      <c r="C41" t="s">
+        <v>33</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+      <c r="K41">
+        <v>0</v>
+      </c>
+      <c r="L41">
+        <v>0</v>
+      </c>
+      <c r="M41">
+        <v>0</v>
+      </c>
+      <c r="N41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
+      <c r="A42">
+        <v>6</v>
+      </c>
+      <c r="B42" t="s">
+        <v>25</v>
+      </c>
+      <c r="C42" t="s">
+        <v>33</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
+      <c r="K42">
+        <v>0</v>
+      </c>
+      <c r="L42">
+        <v>0</v>
+      </c>
+      <c r="M42">
+        <v>0</v>
+      </c>
+      <c r="N42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14">
+      <c r="A43">
+        <v>7</v>
+      </c>
+      <c r="B43" t="s">
+        <v>26</v>
+      </c>
+      <c r="C43" t="s">
+        <v>33</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <v>0</v>
+      </c>
+      <c r="L43">
+        <v>0</v>
+      </c>
+      <c r="M43">
+        <v>0</v>
+      </c>
+      <c r="N43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14">
+      <c r="A44">
+        <v>8</v>
+      </c>
+      <c r="B44" t="s">
+        <v>27</v>
+      </c>
+      <c r="C44" t="s">
+        <v>33</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <v>0</v>
+      </c>
+      <c r="L44">
+        <v>0</v>
+      </c>
+      <c r="M44">
+        <v>0</v>
+      </c>
+      <c r="N44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14">
+      <c r="A45">
+        <v>9</v>
+      </c>
+      <c r="B45" t="s">
+        <v>28</v>
+      </c>
+      <c r="C45" t="s">
+        <v>33</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>0</v>
+      </c>
+      <c r="L45">
+        <v>0</v>
+      </c>
+      <c r="M45">
+        <v>0</v>
+      </c>
+      <c r="N45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14">
+      <c r="A46">
+        <v>21</v>
+      </c>
+      <c r="B46" t="s">
+        <v>29</v>
+      </c>
+      <c r="C46" t="s">
+        <v>33</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+      <c r="K46">
+        <v>0</v>
+      </c>
+      <c r="L46">
+        <v>0</v>
+      </c>
+      <c r="M46">
+        <v>0</v>
+      </c>
+      <c r="N46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14">
+      <c r="A47">
+        <v>22</v>
+      </c>
+      <c r="B47" t="s">
+        <v>30</v>
+      </c>
+      <c r="C47" t="s">
+        <v>33</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+      <c r="K47">
+        <v>0</v>
+      </c>
+      <c r="L47">
+        <v>0</v>
+      </c>
+      <c r="M47">
+        <v>0</v>
+      </c>
+      <c r="N47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14">
+      <c r="A48">
+        <v>23</v>
+      </c>
+      <c r="B48" t="s">
+        <v>31</v>
+      </c>
+      <c r="C48" t="s">
+        <v>33</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+      <c r="K48">
+        <v>0</v>
+      </c>
+      <c r="L48">
+        <v>0</v>
+      </c>
+      <c r="M48">
+        <v>0</v>
+      </c>
+      <c r="N48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14">
+      <c r="A49">
+        <v>24</v>
+      </c>
+      <c r="B49" t="s">
+        <v>32</v>
+      </c>
+      <c r="C49" t="s">
+        <v>33</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49">
+        <v>0</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
+      </c>
+      <c r="K49">
+        <v>0</v>
+      </c>
+      <c r="L49">
+        <v>0</v>
+      </c>
+      <c r="M49">
+        <v>0</v>
+      </c>
+      <c r="N49">
         <v>0</v>
       </c>
     </row>

</xml_diff>